<commit_message>
[Typed SDK] Fix problems found during testing Explorer example
</commit_message>
<xml_diff>
--- a/Runtime/VOSdkTyped/Source/VOSdk/GUI_Classes_SDK/ClassMapping.xlsx
+++ b/Runtime/VOSdkTyped/Source/VOSdk/GUI_Classes_SDK/ClassMapping.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XSharp\DevRt\Runtime\VOSdkTyped\Source\VOSdk\GUI_Classes_SDK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E434D3B1-9768-44BB-810B-9BDBCB41F63C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932E0914-B4E4-4DDD-9B57-390DC143D779}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4683684D-C402-4F2B-ABAA-246EFAFB1186}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{4683684D-C402-4F2B-ABAA-246EFAFB1186}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="List of classes" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -546,9 +546,6 @@
     <t>OnControlCreated, OnHandleCreated, OnHandleDestroyed</t>
   </si>
   <si>
-    <t>Many manye events</t>
-  </si>
-  <si>
     <t>OnControlCreated, RetrieveVirtualItems, CacheVirtualItems, SearchForVirtualItem</t>
   </si>
   <si>
@@ -775,6 +772,9 @@
   </si>
   <si>
     <t>Normally these events or similar events are available for all 3rd party controls as well.</t>
+  </si>
+  <si>
+    <t>Many many events</t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6821692C-EB20-4B92-A7C3-887AABF60203}">
   <dimension ref="A1:A62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
@@ -1146,217 +1146,217 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
@@ -1364,72 +1364,72 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -1441,8 +1441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724AA120-0C83-42E2-87CF-1698B945DC96}">
   <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1603,7 +1603,7 @@
         <v>64</v>
       </c>
       <c r="G12" t="s">
-        <v>170</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1631,7 +1631,7 @@
         <v>63</v>
       </c>
       <c r="G14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1693,7 +1693,7 @@
         <v>24</v>
       </c>
       <c r="G18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1785,19 +1785,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
       </c>
       <c r="C25" t="s">
+        <v>174</v>
+      </c>
+      <c r="D25" t="s">
+        <v>174</v>
+      </c>
+      <c r="G25" t="s">
         <v>175</v>
-      </c>
-      <c r="D25" t="s">
-        <v>175</v>
-      </c>
-      <c r="G25" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1805,7 +1805,7 @@
         <v>97</v>
       </c>
       <c r="B26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C26" t="s">
         <v>70</v>
@@ -1861,31 +1861,31 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1918,7 +1918,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B36" t="s">
         <v>25</v>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B40" t="s">
         <v>31</v>
@@ -2039,7 +2039,7 @@
         <v>11</v>
       </c>
       <c r="G44" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2058,16 +2058,16 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B46" t="s">
         <v>126</v>
       </c>
       <c r="E46" t="s">
+        <v>187</v>
+      </c>
+      <c r="G46" t="s">
         <v>188</v>
-      </c>
-      <c r="G46" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2084,7 +2084,7 @@
         <v>22</v>
       </c>
       <c r="G47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2101,7 +2101,7 @@
         <v>68</v>
       </c>
       <c r="G48" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>